<commit_message>
Use the actual picture resolution
The reference ImageAnchors.xlsx has been updated to match the actual DPI of the SampleImage.jpg file which is 72 DPI but was using 96 DPI.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/ImageHandling/ImageAnchors.xlsx
@@ -212,7 +212,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3810000" cy="3810000"/>
+          <a:ext cx="5080000" cy="5080000"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>
@@ -222,15 +222,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -248,7 +248,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3810000" cy="3810000"/>
+          <a:ext cx="5080000" cy="5080000"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>
@@ -262,7 +262,7 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="762000" cy="762000"/>
+    <xdr:ext cx="1016000" cy="1016000"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 3"/>
@@ -279,7 +279,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="762000" cy="762000"/>
+          <a:ext cx="1016000" cy="1016000"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>
@@ -292,8 +292,8 @@
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
-    <xdr:pos x="952500" y="952500"/>
-    <xdr:ext cx="3810000" cy="3810000"/>
+    <xdr:pos x="1270000" y="1270000"/>
+    <xdr:ext cx="5080000" cy="5080000"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1"/>
@@ -310,7 +310,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3810000" cy="3810000"/>
+          <a:ext cx="5080000" cy="5080000"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>

</xml_diff>